<commit_message>
LC Updated Figures and New Trained Models
</commit_message>
<xml_diff>
--- a/Trained_Models/230204_Models/Model_Selection_compiled.xlsx
+++ b/Trained_Models/230204_Models/Model_Selection_compiled.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\source\repos\ML_LNP\ML_LNP\Trained_Models\230204_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0D197C87-39D9-40AE-A2CA-106937B08DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ADA499-4B5D-4F54-B8CD-0B0A58DC6DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Selection_MAE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>HEK293</t>
   </si>
@@ -75,23 +88,14 @@
   <si>
     <t>average</t>
   </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,8 +573,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -925,11 +930,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,728 +945,765 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>7.6330141344573901E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>6.1257408167824601E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>5.8432347785189E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>8.9882793553645299E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>4.9767856344316803E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>6.0237747419922501E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <f>AVERAGE(B5:G5)</f>
         <v>6.5984715769245347E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.144161604094659</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.12939315303017301</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.12845038995406299</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.17832184196950501</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>9.9993830790113106E-2</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.115067639348182</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <f t="shared" ref="H6:H12" si="0">AVERAGE(B6:G6)</f>
         <v>0.13256474319778253</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.14764647064212999</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.13036957460475199</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0.12682579588033199</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0.18272452512461099</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.100968990351</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.11480878823307</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>0.13389069080598248</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.144159906689872</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.129847763459013</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0.12785555975825499</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0.18428928047399601</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>9.9872309381881699E-2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>0.11477876136373499</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>0.13346726352112545</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0.104406551257269</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>8.0129122053709395E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>8.3739876520952605E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0.105409324931663</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>6.5768890978042893E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>7.8491524236455404E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>8.6324214996348722E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>7.6968655360899099E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>6.1174915454418402E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>6.4839079169875399E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>8.8966972242565195E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>4.8729021283413401E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>6.0216810273258099E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>6.6815908964071594E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>7.4318050397425603E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>6.1583061704565602E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>5.4322910954710903E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>9.2354478679447696E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>4.61450678518023E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>6.1136584060685797E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>6.4976692274772971E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.10029584776199001</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>6.9522321653325198E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>7.6512523267483007E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>0.110830001900104</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>5.96579253938933E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>7.32824869656966E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>8.1683517823748691E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.873526304367783</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>0.79066198000975996</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>0.88010915931573497</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>0.85771242105224899</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>0.90914437285215</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>0.74989703375651595</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <f>AVERAGE(B16:G16)</f>
         <v>0.84350854522569874</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.38282388447408899</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>0.29112105095983798</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>0.51981676872634597</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>0.35233078172503701</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>0.66511655807965797</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>0.59158518558807904</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <f t="shared" ref="H17:H23" si="1">AVERAGE(B17:G17)</f>
         <v>0.46713237159217447</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.40998321900421703</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>0.32118019033481099</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0.504925020323155</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>0.495297502482754</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>0.66488840673886695</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>0.58910320209207701</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <f t="shared" si="1"/>
         <v>0.49756292349598014</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.38274767478670702</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0.34460722757922702</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>0.58805502585963598</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>0.54783872597655303</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>0.66505698853898099</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>0.52409141094506095</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <f t="shared" si="1"/>
         <v>0.50873284228102755</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.71442150515767999</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>0.73178542559217397</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0.81412411640424998</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>0.81073149895325403</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>0.84091639943820995</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>0.674523983247313</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <f t="shared" si="1"/>
         <v>0.76441715479881356</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.84743445743798496</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>0.78875137125075201</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>0.87031793620917797</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>0.86518500300934098</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>0.91822018553603901</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>0.75884495452662903</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <f t="shared" si="1"/>
         <v>0.84145898466165414</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.861135100265082</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>0.79614008195082597</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>0.89233169768784004</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>0.86053690524348103</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.90299917903595195</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>0.75636595705504595</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <f t="shared" si="1"/>
         <v>0.84491815353970434</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.74627351795416597</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.58297474472947297</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>0.83271396327079195</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>0.82738760852675497</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.87066503768186398</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>0.71752500867837798</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <f t="shared" si="1"/>
         <v>0.76292331347357134</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0.85679434436811197</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>0.89739853346313103</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>0.88144749023819302</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>0.86252497374970605</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>0.92426186793507203</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>0.90152674517704501</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="1">
         <f>AVERAGE(B27:G27)</f>
         <v>0.88732565915520978</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.36736321260138199</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>0.42882294638336599</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>0.49510617405927698</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>0.38351237955434397</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>0.67540602909830405</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>0.64523503753085698</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <f t="shared" ref="H28:H34" si="2">AVERAGE(B28:G28)</f>
         <v>0.49924096320458838</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.36672603261155801</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>0.37112580580336901</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>0.447352864332902</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>0.47823041750468198</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>0.67328156399947003</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>0.647107629253456</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <f t="shared" si="2"/>
         <v>0.49730405225090618</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0.36732272860401899</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>0.37673880430388501</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>0.51257842449288404</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>0.51143332891814397</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>0.67585305411964702</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>0.66540088897680205</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1">
         <f t="shared" si="2"/>
         <v>0.51822120490256351</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>0.70616969635397897</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>0.83240294734585096</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>0.80221295861998898</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>0.78294721319182803</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>0.858777794476417</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>0.84806171531460794</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <f t="shared" si="2"/>
         <v>0.8050953875504453</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>0.84808835143662298</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>0.92816035397389096</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>0.89123146161066302</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>0.87235913370231299</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>0.93952188922232005</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>0.89920540477077604</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <f t="shared" si="2"/>
         <v>0.89642776578609773</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>0.84992632568443505</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>0.89510473870981599</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>0.91675466848055898</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>0.85970187425653999</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>0.92656568454940502</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>0.90603894357844605</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <f t="shared" si="2"/>
         <v>0.89234870587653348</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>0.74131428870974803</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>0.78931208338058301</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>0.78560151477917795</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>0.815350440522006</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>0.89276885248287197</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>0.876613507039955</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <f t="shared" si="2"/>
         <v>0.81682678115239027</v>
       </c>

</xml_diff>